<commit_message>
removed db and mig
</commit_message>
<xml_diff>
--- a/docs/Project Management/work log.xlsx
+++ b/docs/Project Management/work log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="27720" tabRatio="500" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Current Functionality" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="419">
   <si>
     <t>Project Name</t>
   </si>
@@ -1414,12 +1414,18 @@
   <si>
     <t>Zulu</t>
   </si>
+  <si>
+    <t xml:space="preserve">not all experiments are showing for participants </t>
+  </si>
+  <si>
+    <t>Languages' object has no attribute 'lower'</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1506,6 +1512,11 @@
       <vertAlign val="superscript"/>
       <sz val="12"/>
       <name val="Consolas"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1615,7 +1626,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1670,6 +1681,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3264,10 +3276,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3306,6 +3318,14 @@
     <row r="2" spans="1:15">
       <c r="A2">
         <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="21">
+      <c r="C3" s="24" t="s">
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -4819,7 +4839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B95" sqref="B1:B95"/>
     </sheetView>
   </sheetViews>

</xml_diff>